<commit_message>
shit ton of fixes
</commit_message>
<xml_diff>
--- a/files/resultados/2023/resultados_2023.xlsx
+++ b/files/resultados/2023/resultados_2023.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="186">
   <si>
     <t>res_c1</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t>_uuid</t>
+  </si>
+  <si>
+    <t>cri_p2_c3</t>
   </si>
   <si>
     <t>Alcaldia Local De Antonio Narino</t>
@@ -926,13 +929,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AS71"/>
+  <dimension ref="A1:AT71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:45">
+    <row r="1" spans="1:46">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1068,8 +1071,11 @@
       <c r="AS1" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="AT1" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="2" spans="1:45">
+    <row r="2" spans="1:46">
       <c r="A2">
         <v>16</v>
       </c>
@@ -1089,7 +1095,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -1203,10 +1209,10 @@
         <v>0</v>
       </c>
       <c r="AS2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:45">
+    <row r="3" spans="1:46">
       <c r="A3">
         <v>42.40000000000001</v>
       </c>
@@ -1226,7 +1232,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -1340,10 +1346,10 @@
         <v>0</v>
       </c>
       <c r="AS3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:45">
+    <row r="4" spans="1:46">
       <c r="A4">
         <v>39.88</v>
       </c>
@@ -1363,7 +1369,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -1477,10 +1483,10 @@
         <v>0</v>
       </c>
       <c r="AS4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:45">
+    <row r="5" spans="1:46">
       <c r="A5">
         <v>46.88</v>
       </c>
@@ -1500,7 +1506,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -1614,10 +1620,10 @@
         <v>0</v>
       </c>
       <c r="AS5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:45">
+    <row r="6" spans="1:46">
       <c r="A6">
         <v>23.2</v>
       </c>
@@ -1637,7 +1643,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -1751,10 +1757,10 @@
         <v>0</v>
       </c>
       <c r="AS6" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:45">
+    <row r="7" spans="1:46">
       <c r="A7">
         <v>13</v>
       </c>
@@ -1774,7 +1780,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -1888,10 +1894,10 @@
         <v>0</v>
       </c>
       <c r="AS7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:45">
+    <row r="8" spans="1:46">
       <c r="A8">
         <v>37.8</v>
       </c>
@@ -1911,7 +1917,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -2025,10 +2031,10 @@
         <v>0</v>
       </c>
       <c r="AS8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:45">
+    <row r="9" spans="1:46">
       <c r="A9">
         <v>28.4</v>
       </c>
@@ -2048,7 +2054,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -2162,10 +2168,10 @@
         <v>0</v>
       </c>
       <c r="AS9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:45">
+    <row r="10" spans="1:46">
       <c r="A10">
         <v>32.6</v>
       </c>
@@ -2185,7 +2191,7 @@
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -2299,10 +2305,10 @@
         <v>0</v>
       </c>
       <c r="AS10" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:45">
+    <row r="11" spans="1:46">
       <c r="A11">
         <v>26.4</v>
       </c>
@@ -2322,7 +2328,7 @@
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -2436,10 +2442,10 @@
         <v>0</v>
       </c>
       <c r="AS11" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
-    <row r="12" spans="1:45">
+    <row r="12" spans="1:46">
       <c r="A12">
         <v>36.8</v>
       </c>
@@ -2459,7 +2465,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -2573,10 +2579,10 @@
         <v>0</v>
       </c>
       <c r="AS12" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
-    <row r="13" spans="1:45">
+    <row r="13" spans="1:46">
       <c r="A13">
         <v>24.2</v>
       </c>
@@ -2596,7 +2602,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -2710,10 +2716,10 @@
         <v>0</v>
       </c>
       <c r="AS13" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
-    <row r="14" spans="1:45">
+    <row r="14" spans="1:46">
       <c r="A14">
         <v>0</v>
       </c>
@@ -2733,7 +2739,7 @@
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -2847,10 +2853,10 @@
         <v>0</v>
       </c>
       <c r="AS14" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:45">
+    <row r="15" spans="1:46">
       <c r="A15">
         <v>34</v>
       </c>
@@ -2870,7 +2876,7 @@
         <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -2984,10 +2990,10 @@
         <v>0</v>
       </c>
       <c r="AS15" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
-    <row r="16" spans="1:45">
+    <row r="16" spans="1:46">
       <c r="A16">
         <v>47.2</v>
       </c>
@@ -3007,7 +3013,7 @@
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -3121,7 +3127,7 @@
         <v>0</v>
       </c>
       <c r="AS16" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:45">
@@ -3144,7 +3150,7 @@
         <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -3258,7 +3264,7 @@
         <v>0</v>
       </c>
       <c r="AS17" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:45">
@@ -3281,7 +3287,7 @@
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -3395,7 +3401,7 @@
         <v>0</v>
       </c>
       <c r="AS18" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" spans="1:45">
@@ -3418,7 +3424,7 @@
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -3532,7 +3538,7 @@
         <v>0</v>
       </c>
       <c r="AS19" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:45">
@@ -3555,7 +3561,7 @@
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -3669,7 +3675,7 @@
         <v>0</v>
       </c>
       <c r="AS20" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="21" spans="1:45">
@@ -3692,7 +3698,7 @@
         <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -3806,7 +3812,7 @@
         <v>0</v>
       </c>
       <c r="AS21" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22" spans="1:45">
@@ -3829,7 +3835,7 @@
         <v>0</v>
       </c>
       <c r="G22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H22">
         <v>0</v>
@@ -3943,7 +3949,7 @@
         <v>0</v>
       </c>
       <c r="AS22" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:45">
@@ -3966,7 +3972,7 @@
         <v>0</v>
       </c>
       <c r="G23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -4080,7 +4086,7 @@
         <v>0</v>
       </c>
       <c r="AS23" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:45">
@@ -4094,7 +4100,7 @@
         <v>0</v>
       </c>
       <c r="G24" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H24">
         <v>0</v>
@@ -4208,7 +4214,7 @@
         <v>0</v>
       </c>
       <c r="AS24" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:45">
@@ -4231,7 +4237,7 @@
         <v>0</v>
       </c>
       <c r="G25" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -4345,7 +4351,7 @@
         <v>0</v>
       </c>
       <c r="AS25" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26" spans="1:45">
@@ -4368,7 +4374,7 @@
         <v>0</v>
       </c>
       <c r="G26" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H26">
         <v>0</v>
@@ -4482,7 +4488,7 @@
         <v>0</v>
       </c>
       <c r="AS26" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="27" spans="1:45">
@@ -4496,7 +4502,7 @@
         <v>0</v>
       </c>
       <c r="G27" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H27">
         <v>0</v>
@@ -4610,7 +4616,7 @@
         <v>0</v>
       </c>
       <c r="AS27" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" spans="1:45">
@@ -4633,7 +4639,7 @@
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H28">
         <v>0</v>
@@ -4747,7 +4753,7 @@
         <v>0</v>
       </c>
       <c r="AS28" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29" spans="1:45">
@@ -4770,7 +4776,7 @@
         <v>0</v>
       </c>
       <c r="G29" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H29">
         <v>0</v>
@@ -4884,7 +4890,7 @@
         <v>0</v>
       </c>
       <c r="AS29" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:45">
@@ -4907,7 +4913,7 @@
         <v>0</v>
       </c>
       <c r="G30" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H30">
         <v>0</v>
@@ -5021,7 +5027,7 @@
         <v>0</v>
       </c>
       <c r="AS30" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="31" spans="1:45">
@@ -5044,7 +5050,7 @@
         <v>0</v>
       </c>
       <c r="G31" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -5158,7 +5164,7 @@
         <v>0</v>
       </c>
       <c r="AS31" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="32" spans="1:45">
@@ -5181,7 +5187,7 @@
         <v>0</v>
       </c>
       <c r="G32" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H32">
         <v>0</v>
@@ -5295,7 +5301,7 @@
         <v>0</v>
       </c>
       <c r="AS32" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="33" spans="1:45">
@@ -5318,7 +5324,7 @@
         <v>0</v>
       </c>
       <c r="G33" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H33">
         <v>0</v>
@@ -5432,7 +5438,7 @@
         <v>0</v>
       </c>
       <c r="AS33" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="34" spans="1:45">
@@ -5455,7 +5461,7 @@
         <v>0</v>
       </c>
       <c r="G34" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H34">
         <v>0</v>
@@ -5569,7 +5575,7 @@
         <v>0</v>
       </c>
       <c r="AS34" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="35" spans="1:45">
@@ -5592,7 +5598,7 @@
         <v>0</v>
       </c>
       <c r="G35" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H35">
         <v>0</v>
@@ -5706,7 +5712,7 @@
         <v>0</v>
       </c>
       <c r="AS35" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="36" spans="1:45">
@@ -5729,7 +5735,7 @@
         <v>0</v>
       </c>
       <c r="G36" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H36">
         <v>0</v>
@@ -5843,7 +5849,7 @@
         <v>0</v>
       </c>
       <c r="AS36" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="37" spans="1:45">
@@ -5866,7 +5872,7 @@
         <v>0</v>
       </c>
       <c r="G37" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H37">
         <v>0</v>
@@ -5980,7 +5986,7 @@
         <v>0</v>
       </c>
       <c r="AS37" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="38" spans="1:45">
@@ -6003,7 +6009,7 @@
         <v>0</v>
       </c>
       <c r="G38" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H38">
         <v>0</v>
@@ -6117,7 +6123,7 @@
         <v>0</v>
       </c>
       <c r="AS38" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="39" spans="1:45">
@@ -6140,7 +6146,7 @@
         <v>0</v>
       </c>
       <c r="G39" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H39">
         <v>0</v>
@@ -6254,7 +6260,7 @@
         <v>0</v>
       </c>
       <c r="AS39" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="40" spans="1:45">
@@ -6277,7 +6283,7 @@
         <v>0</v>
       </c>
       <c r="G40" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H40">
         <v>0</v>
@@ -6391,7 +6397,7 @@
         <v>0</v>
       </c>
       <c r="AS40" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="41" spans="1:45">
@@ -6414,7 +6420,7 @@
         <v>0</v>
       </c>
       <c r="G41" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H41">
         <v>0</v>
@@ -6528,7 +6534,7 @@
         <v>0</v>
       </c>
       <c r="AS41" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="42" spans="1:45">
@@ -6551,7 +6557,7 @@
         <v>0</v>
       </c>
       <c r="G42" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H42">
         <v>0</v>
@@ -6665,7 +6671,7 @@
         <v>0</v>
       </c>
       <c r="AS42" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="43" spans="1:45">
@@ -6688,7 +6694,7 @@
         <v>0</v>
       </c>
       <c r="G43" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H43">
         <v>0</v>
@@ -6802,7 +6808,7 @@
         <v>0</v>
       </c>
       <c r="AS43" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="44" spans="1:45">
@@ -6825,7 +6831,7 @@
         <v>0</v>
       </c>
       <c r="G44" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H44">
         <v>0</v>
@@ -6939,7 +6945,7 @@
         <v>0</v>
       </c>
       <c r="AS44" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="45" spans="1:45">
@@ -6962,7 +6968,7 @@
         <v>0</v>
       </c>
       <c r="G45" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H45">
         <v>0</v>
@@ -7076,7 +7082,7 @@
         <v>0</v>
       </c>
       <c r="AS45" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="46" spans="1:45">
@@ -7099,7 +7105,7 @@
         <v>0</v>
       </c>
       <c r="G46" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H46">
         <v>0</v>
@@ -7213,7 +7219,7 @@
         <v>0</v>
       </c>
       <c r="AS46" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="47" spans="1:45">
@@ -7236,7 +7242,7 @@
         <v>0</v>
       </c>
       <c r="G47" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H47">
         <v>0</v>
@@ -7350,7 +7356,7 @@
         <v>0</v>
       </c>
       <c r="AS47" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="48" spans="1:45">
@@ -7373,7 +7379,7 @@
         <v>0</v>
       </c>
       <c r="G48" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H48">
         <v>0</v>
@@ -7487,7 +7493,7 @@
         <v>0</v>
       </c>
       <c r="AS48" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="49" spans="1:45">
@@ -7510,7 +7516,7 @@
         <v>0</v>
       </c>
       <c r="G49" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H49">
         <v>0</v>
@@ -7624,7 +7630,7 @@
         <v>0</v>
       </c>
       <c r="AS49" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="50" spans="1:45">
@@ -7647,7 +7653,7 @@
         <v>0</v>
       </c>
       <c r="G50" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H50">
         <v>0</v>
@@ -7761,7 +7767,7 @@
         <v>0</v>
       </c>
       <c r="AS50" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="51" spans="1:45">
@@ -7784,7 +7790,7 @@
         <v>0</v>
       </c>
       <c r="G51" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H51">
         <v>0</v>
@@ -7898,7 +7904,7 @@
         <v>0</v>
       </c>
       <c r="AS51" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="52" spans="1:45">
@@ -7921,7 +7927,7 @@
         <v>0</v>
       </c>
       <c r="G52" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H52">
         <v>0</v>
@@ -8035,7 +8041,7 @@
         <v>0</v>
       </c>
       <c r="AS52" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="53" spans="1:45">
@@ -8058,7 +8064,7 @@
         <v>0</v>
       </c>
       <c r="G53" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H53">
         <v>0</v>
@@ -8172,7 +8178,7 @@
         <v>0</v>
       </c>
       <c r="AS53" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="54" spans="1:45">
@@ -8195,7 +8201,7 @@
         <v>0</v>
       </c>
       <c r="G54" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H54">
         <v>0</v>
@@ -8309,7 +8315,7 @@
         <v>0</v>
       </c>
       <c r="AS54" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="55" spans="1:45">
@@ -8332,7 +8338,7 @@
         <v>0</v>
       </c>
       <c r="G55" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H55">
         <v>0</v>
@@ -8446,7 +8452,7 @@
         <v>0</v>
       </c>
       <c r="AS55" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="56" spans="1:45">
@@ -8469,7 +8475,7 @@
         <v>0</v>
       </c>
       <c r="G56" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H56">
         <v>0</v>
@@ -8583,7 +8589,7 @@
         <v>0</v>
       </c>
       <c r="AS56" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="57" spans="1:45">
@@ -8606,7 +8612,7 @@
         <v>0</v>
       </c>
       <c r="G57" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H57">
         <v>0</v>
@@ -8720,7 +8726,7 @@
         <v>0</v>
       </c>
       <c r="AS57" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="58" spans="1:45">
@@ -8743,7 +8749,7 @@
         <v>0</v>
       </c>
       <c r="G58" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H58">
         <v>0</v>
@@ -8857,7 +8863,7 @@
         <v>0</v>
       </c>
       <c r="AS58" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="59" spans="1:45">
@@ -8880,7 +8886,7 @@
         <v>0</v>
       </c>
       <c r="G59" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H59">
         <v>0</v>
@@ -8994,7 +9000,7 @@
         <v>0</v>
       </c>
       <c r="AS59" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="60" spans="1:45">
@@ -9017,7 +9023,7 @@
         <v>0</v>
       </c>
       <c r="G60" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H60">
         <v>0</v>
@@ -9131,7 +9137,7 @@
         <v>0</v>
       </c>
       <c r="AS60" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="61" spans="1:45">
@@ -9154,7 +9160,7 @@
         <v>0</v>
       </c>
       <c r="G61" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H61">
         <v>0</v>
@@ -9268,7 +9274,7 @@
         <v>0</v>
       </c>
       <c r="AS61" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="62" spans="1:45">
@@ -9291,7 +9297,7 @@
         <v>0</v>
       </c>
       <c r="G62" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H62">
         <v>0</v>
@@ -9405,7 +9411,7 @@
         <v>0</v>
       </c>
       <c r="AS62" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="63" spans="1:45">
@@ -9428,7 +9434,7 @@
         <v>0</v>
       </c>
       <c r="G63" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H63">
         <v>0</v>
@@ -9542,7 +9548,7 @@
         <v>0</v>
       </c>
       <c r="AS63" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="64" spans="1:45">
@@ -9565,7 +9571,7 @@
         <v>0</v>
       </c>
       <c r="G64" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H64">
         <v>0</v>
@@ -9679,7 +9685,7 @@
         <v>0</v>
       </c>
       <c r="AS64" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="65" spans="1:45">
@@ -9693,7 +9699,7 @@
         <v>0</v>
       </c>
       <c r="G65" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H65">
         <v>0</v>
@@ -9807,7 +9813,7 @@
         <v>0</v>
       </c>
       <c r="AS65" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="66" spans="1:45">
@@ -9830,7 +9836,7 @@
         <v>0</v>
       </c>
       <c r="G66" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H66">
         <v>0</v>
@@ -9944,7 +9950,7 @@
         <v>0</v>
       </c>
       <c r="AS66" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="67" spans="1:45">
@@ -9967,7 +9973,7 @@
         <v>0</v>
       </c>
       <c r="G67" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H67">
         <v>0</v>
@@ -10081,7 +10087,7 @@
         <v>0</v>
       </c>
       <c r="AS67" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="68" spans="1:45">
@@ -10104,7 +10110,7 @@
         <v>0</v>
       </c>
       <c r="G68" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H68">
         <v>0</v>
@@ -10218,7 +10224,7 @@
         <v>0</v>
       </c>
       <c r="AS68" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="69" spans="1:45">
@@ -10241,7 +10247,7 @@
         <v>0</v>
       </c>
       <c r="G69" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H69">
         <v>0</v>
@@ -10355,7 +10361,7 @@
         <v>0</v>
       </c>
       <c r="AS69" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="70" spans="1:45">
@@ -10378,7 +10384,7 @@
         <v>0</v>
       </c>
       <c r="G70" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H70">
         <v>0</v>
@@ -10492,7 +10498,7 @@
         <v>0</v>
       </c>
       <c r="AS70" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="71" spans="1:45">
@@ -10515,7 +10521,7 @@
         <v>0</v>
       </c>
       <c r="G71" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H71">
         <v>0</v>
@@ -10629,7 +10635,7 @@
         <v>0</v>
       </c>
       <c r="AS71" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
git commit calificacion hasta p23
</commit_message>
<xml_diff>
--- a/files/resultados/2023/resultados_2023.xlsx
+++ b/files/resultados/2023/resultados_2023.xlsx
@@ -5521,7 +5521,7 @@
         <v>0</v>
       </c>
       <c r="AB34">
-        <v>5.6</v>
+        <v>0</v>
       </c>
       <c r="AC34">
         <v>0</v>
@@ -5569,7 +5569,7 @@
         <v>0</v>
       </c>
       <c r="AR34">
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="AS34" t="s">
         <v>147</v>

</xml_diff>

<commit_message>
||BETA 1.2|| Se añade Dockerfile en detached
</commit_message>
<xml_diff>
--- a/files/resultados/2023/resultados_2023.xlsx
+++ b/files/resultados/2023/resultados_2023.xlsx
@@ -4672,7 +4672,7 @@
         <v>0.6</v>
       </c>
       <c r="U30" t="n">
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
       <c r="V30" t="n">
         <v>0.55</v>
@@ -4693,13 +4693,13 @@
         <v>0.4</v>
       </c>
       <c r="AB30" t="n">
-        <v>1.01</v>
+        <v>3.28</v>
       </c>
       <c r="AC30" t="n">
         <v>0</v>
       </c>
       <c r="AD30" t="n">
-        <v>2.2</v>
+        <v>1</v>
       </c>
       <c r="AE30" t="n">
         <v>1</v>
@@ -4708,7 +4708,7 @@
         <v>0</v>
       </c>
       <c r="AG30" t="n">
-        <v>8.199999999999999</v>
+        <v>13.1</v>
       </c>
       <c r="AH30" t="n">
         <v>1.1</v>

</xml_diff>